<commit_message>
Veyer and POD updates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcsweeney\Desktop\UiDemo Testing\RPA Vendor Dispute Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37970D11-9E89-4013-852B-4C45D14DF1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE8B29-88B8-4384-A607-BDA8C602CF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24405" yWindow="1830" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
   <si>
     <t>Name</t>
   </si>
@@ -101,10 +101,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -441,27 +437,6 @@
     <t>Vendor_Dispute_Queue_POD</t>
   </si>
   <si>
-    <t>Vendor_Dispute_Queue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successful | Dispute &amp; POD Bot |  </t>
-  </si>
-  <si>
-    <t>ExceptionBatchMailSubject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exception | Dispute &amp; POD Bot |  </t>
-  </si>
-  <si>
-    <t>UploaderIssueMailSubject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial Successful | Dispute &amp; POD Bot | </t>
-  </si>
-  <si>
-    <t>BottyExceptionMailSubject</t>
-  </si>
-  <si>
     <t>SystemExceptionMailRecipients</t>
   </si>
   <si>
@@ -517,99 +492,435 @@
   </si>
   <si>
     <t>Recipients</t>
+  </si>
+  <si>
+    <t>SuccessDisputeMailBody</t>
+  </si>
+  <si>
+    <t>SuccessDisputeMailSubject</t>
+  </si>
+  <si>
+    <t>ArchiveSavedBatch</t>
+  </si>
+  <si>
+    <t>TransactionUploaderRequestName</t>
+  </si>
+  <si>
+    <t>TransactionUploaderFileUploadName</t>
+  </si>
+  <si>
+    <t>Oracle_Credential</t>
+  </si>
+  <si>
+    <t>Oracle_Claim_Credentials</t>
+  </si>
+  <si>
+    <t>JavaFilePath</t>
+  </si>
+  <si>
+    <t>C:\Program Files\Java\jre1.8.0_431\bin\jp2launcher.exe</t>
+  </si>
+  <si>
+    <t>TargetAsanaUserID</t>
+  </si>
+  <si>
+    <t>&lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Dear Team,&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Please find below the &lt;strong&gt;Validation Summary&lt;/strong&gt; of the claims processed in File:&lt;strong&gt; {9} &lt;/strong&gt;for &lt;strong&gt;{10}&lt;/strong&gt;:&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Uploader Step:&lt;/strong&gt; Error Occured in the creation and running the CSV file for Claim Uploader. This step will need to be completed manually, please contact IT to get an understanding of the exception&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Uploader ID:&lt;/strong&gt; {12}&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Send to Botty Step:&lt;/strong&gt; Step skipped due to exception in Uploader step&lt;/p&gt; 
+    &lt;table border='0' cellpadding='8' cellspacing='0' style='border-collapse: collapse; width: 60%; font-family: Arial, sans-serif; font-size: 14px;'&gt; 
+    &lt;thead&gt; 
+    &lt;tr style='background-color: #4CAF50; color: white;'&gt; 
+    &lt;th style='border: 1px solid #ddd;'&gt;Metric&lt;/th&gt;&lt;th style='border: 1px solid #ddd;'&gt;Count&lt;/th&gt; 
+    &lt;/tr&gt; 
+    &lt;/thead&gt; 
+&lt;tbody&gt; 
+              &lt;td style='border: 1px solid #ddd;'&gt;Claim Not Open/Claim Not Found&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{0}&lt;/td&gt;
+        &lt;/tr&gt; 
+       &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Backup Not Open&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{1}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Validation Exception&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{2}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Accrual Issue&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{3}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Inactive Offer&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{4}&lt;/td&gt;
+        &lt;/tr&gt; 
+  &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Uploader Exception&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{5}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Issue Adding to Botty File&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{6}&lt;/td&gt;
+        &lt;/tr&gt; 
+      &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Sent to Botty for Submission&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{7}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+        &lt;tr style='background-color: #f1f1f1; font-weight: bold;'&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Total&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{8}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;/tbody&gt;     &lt;/table&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Regards,&lt;br/&gt;RPA Bot&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>POD-BottyExceptionMailBody</t>
+  </si>
+  <si>
+    <t>POD-BottyExceptionMailSubject</t>
+  </si>
+  <si>
+    <t>POD-UploaderIssueMailBody</t>
+  </si>
+  <si>
+    <t>POD-UploaderIssueMailSubject</t>
+  </si>
+  <si>
+    <t>POD-SuccessMailBody</t>
+  </si>
+  <si>
+    <t>POD-SuccessBatchMailSubject</t>
+  </si>
+  <si>
+    <t>&lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Dear Team,&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Please find below the &lt;strong&gt;POD Process Summary&lt;/strong&gt; of the claims processed in this bot run.&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Uploader Step:&lt;/strong&gt; {11}&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Uploader ID:&lt;/strong&gt; {12}&lt;/p&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;&lt;strong&gt;Send to Botty Step:&lt;/strong&gt;Error Occured in the creation and moving of the Botty Files. This step will need to be completed manually, please contact IT to get an understanding of the exception&lt;/p&gt; 
+    &lt;table border='0' cellpadding='8' cellspacing='0' style='border-collapse: collapse; width: 60%; font-family: Arial, sans-serif; font-size: 14px;'&gt; 
+    &lt;thead&gt; 
+    &lt;tr style='background-color: #4CAF50; color: white;'&gt; 
+    &lt;th style='border: 1px solid #ddd;'&gt;Metric&lt;/th&gt;&lt;th style='border: 1px solid #ddd;'&gt;Count&lt;/th&gt; 
+    &lt;/tr&gt; 
+    &lt;/thead&gt; 
+    &lt;tbody&gt; 
+              &lt;td style='border: 1px solid #ddd;'&gt;Existing Claims Updated on Tracker&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{0}&lt;/td&gt;
+        &lt;/tr&gt; 
+       &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Existing Claims to be CB&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{1}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Existing Claims to be Credited&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{2}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Total New POD Claims&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{3}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Inactive Offer&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{4}&lt;/td&gt;
+        &lt;/tr&gt; 
+  &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Uploader Exception&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{5}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Issue Adding to Botty File&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{6}&lt;/td&gt;
+        &lt;/tr&gt; 
+      &lt;tr&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Sent to Botty for Submission&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{7}&lt;/td&gt;
+        &lt;/tr&gt; 
+        &lt;tr&gt; 
+        &lt;tr style='background-color: #f1f1f1; font-weight: bold;'&gt; 
+            &lt;td style='border: 1px solid #ddd;'&gt;Total&lt;/td&gt;
+            &lt;td style='border: 1px solid #ddd;'&gt;{8}&lt;/td&gt;
+        &lt;/tr&gt; 
+    &lt;/tbody&gt; 
+    &lt;/table&gt; 
+    &lt;p style='font-family: Arial, sans-serif; font-size: 14px;'&gt;Regards,&lt;br/&gt;RPA Bot&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>StaplesFileLocation</t>
+  </si>
+  <si>
+    <t>C:\Users\amcsweeney\Downloads\dSIPUTE bOT fOLDER\Paid Invoices_Debit Credit Memo Export.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful | Claims POD Bot |  </t>
   </si>
   <si>
     <t>&lt;!DOCTYPE html&gt;
 &lt;html&gt;
 &lt;head&gt;
 &lt;style&gt;
-  body {
-    font-family: Arial, sans-serif;
-    font-size: 14px;
-    color: #333333;
-    line-height: 1.5;
-  }
-  .table-container {
-    margin-top: 15px;
-    margin-bottom: 20px;
-  }
-  table {
-    border-collapse: collapse;
-    width: 400px; /* Fixed width for a compact look like your image */
-    font-size: 13px;
-  }
-  th {
-    background-color: #f2f2f2;
-    text-align: left;
-    font-weight: bold;
-    padding: 8px;
-    border: 1px solid #999999;
-  }
-  td {
-    padding: 8px;
-    border: 1px solid #999999;
-  }
-  .count-col {
-    width: 80px;
-    text-align: center;
-  }
+    body { font-family: Arial, sans-serif; color: #333; line-height: 1.6; }
+    .container { width: 85%; margin: 20px auto; border: 1px solid #ddd; padding: 20px; border-radius: 8px; }
+    .header-text { font-size: 14px; margin-bottom: 15px; }
+    .status-box { background-color: #fcf8e3; border: 1px solid #faebcc; color: #8a6d3b; padding: 12px; margin: 15px 0; border-radius: 4px; }
+    table { width: 100%; border-collapse: collapse; margin: 15px 0; }
+    th, td { border: 1px solid #ddd; padding: 10px; text-align: left; font-size: 14px; }
+    th { background-color: #f2f2f2; font-weight: bold; }
+    .section-title { font-size: 16px; font-weight: bold; margin-top: 20px; display: flex; align-items: center; }
+    .footer { font-size: 12px; color: #777; margin-top: 25px; border-top: 1px solid #eee; padding-top: 10px; }
+&lt;/style&gt;
+&lt;/head&gt;
+&lt;body&gt;
+    &lt;div class="container"&gt;
+        &lt;p class="header-text"&gt;Please find below the &lt;strong&gt;POD Process Summary&lt;/strong&gt; of the claims processed in this bot run.&lt;/p&gt;
+        &lt;p class="header-text"&gt;&lt;strong&gt;Uploader Step:&lt;/strong&gt; {Uploader_Step}&lt;/p&gt;
+        &lt;p class="header-text"&gt;&lt;strong&gt;Uploader ID:&lt;/strong&gt; {Uploader_ID}&lt;/p&gt;
+       &lt;p class="header-text"&gt;&lt;strong&gt;Send to Botty Step:&lt;/strong&gt; {Botty_Status_Message}
+      &lt;/p&gt;
+        &lt;hr style="border: 0; border-top: 1px solid #eee;"&gt;
+        &lt;div class="section-title"&gt;📊 Volume Overview&lt;/div&gt;
+        &lt;table&gt;
+            &lt;thead&gt;
+                &lt;tr&gt;
+                    &lt;th&gt;Category&lt;/th&gt;
+                    &lt;th&gt;Volume&lt;/th&gt;
+                    &lt;th&gt;Percentage&lt;/th&gt;
+                &lt;/tr&gt;
+            &lt;/thead&gt;
+            &lt;tbody&gt;
+                &lt;tr&gt;
+                    &lt;td&gt;&lt;strong&gt;Total PODs Processed&lt;/strong&gt;&lt;/td&gt;
+                    &lt;td&gt;{Total_Count}&lt;/td&gt;
+                    &lt;td&gt;100%&lt;/td&gt;
+                &lt;/tr&gt;
+                &lt;tr&gt;
+                    &lt;td&gt;&lt;strong&gt;Existing PODs Updated&lt;/strong&gt;&lt;/td&gt;
+                    &lt;td&gt;{Existing_Count}&lt;/td&gt;
+                    &lt;td&gt;{Existing_Percent}%&lt;/td&gt;
+                &lt;/tr&gt;
+                &lt;tr&gt;
+                    &lt;td&gt;&lt;strong&gt;New PODs Created&lt;/strong&gt;&lt;/td&gt;
+                    &lt;td&gt;{New_Count}&lt;/td&gt;
+                    &lt;td&gt;{New_Percent}%&lt;/td&gt;
+                &lt;/tr&gt;
+            &lt;/tbody&gt;
+        &lt;/table&gt;
+        &lt;div class="section-title"&gt;🔍 Process Breakdown&lt;/div&gt;
+        &lt;table&gt;
+            &lt;thead&gt;
+                &lt;tr&gt;
+                    &lt;th&gt;Logic Group&lt;/th&gt;
+                    &lt;th&gt;Outcome Description&lt;/th&gt;
+                    &lt;th&gt;Count&lt;/th&gt;
+                &lt;/tr&gt;
+            &lt;/thead&gt;
+            &lt;tbody&gt;
+                &lt;tr&gt;
+                    &lt;td rowspan="2"&gt;&lt;strong&gt;New POD Creation&lt;/strong&gt;&lt;/td&gt;
+                    &lt;td&gt;Tasks Created (DM Found)&lt;/td&gt;
+                    &lt;td&gt;{New_Success_Count}&lt;/td&gt;
+                &lt;/tr&gt;
+                &lt;tr&gt;
+                    &lt;td&gt;Tasks Pending (DM Missing)&lt;/td&gt;
+                    &lt;td&gt;{New_Fail_Count}&lt;/td&gt;
+                &lt;/tr&gt;
+                &lt;tr&gt;
+                    &lt;td rowspan="2"&gt;&lt;strong&gt;Data Sync (Existing)&lt;/strong&gt;&lt;/td&gt;
+                    &lt;td&gt;Successful Updates&lt;/td&gt;
+                    &lt;td&gt;{Sync_Success_Count}&lt;/td&gt;
+                &lt;/tr&gt;
+                &lt;tr&gt;
+                    &lt;td&gt;Updates with Errors&lt;/td&gt;
+                    &lt;td&gt;{Sync_Fail_Count}&lt;/td&gt;
+                &lt;/tr&gt;
+            &lt;/tbody&gt;
+        &lt;/table&gt;
+        &lt;div class="footer"&gt;
+            &lt;p&gt;This is an automated report generated by the UiPath POD Automation Robot.&lt;/p&gt;
+        &lt;/div&gt;
+    &lt;/div&gt;
+&lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Successful - Uploader | Claims POD Bot | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Successful - Botty File | Claims POD Bot | </t>
+  </si>
+  <si>
+    <t>UploaderDisputeMailSubject</t>
+  </si>
+  <si>
+    <t>UploaderDisputeMailBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Successful - Uploader | Dispute Bot |  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful | Dispute Bot |  </t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html&gt;
+&lt;head&gt;
+&lt;style&gt;
+  body { font-family: Arial, sans-serif; font-size: 14px; color: #333333; line-height: 1.5; }
+  .table-container { margin-top: 15px; margin-bottom: 20px; }
+  table { border-collapse: collapse; width: 450px; font-size: 13px; }
+  th { background-color: #f2f2f2; text-align: left; font-weight: bold; padding: 8px; border: 1px solid #999999; }
+  td { padding: 8px; border: 1px solid #999999; }
+  .count-col { width: 100px; text-align: center; }
+  .status-text { font-family: Arial, sans-serif; font-size: 14px; margin: 10px 0; }
 &lt;/style&gt;
 &lt;/head&gt;
 &lt;body&gt;
 &lt;p&gt;Hi Team,&lt;/p&gt;
-&lt;p&gt;The &lt;strong&gt;Dispute Customer Portal&lt;/strong&gt; submission process has completed.&lt;br&gt;
-Please find the attachment of the consolidated log table for your reference.&lt;/p&gt;
+&lt;p class="status-text"&gt;Please find below the &lt;strong&gt;Dispute Process Summary&lt;/strong&gt; of the claims processed in this bot run.&lt;/p&gt; 
+&lt;p class="status-text"&gt;&lt;strong&gt;Uploader Step:&lt;/strong&gt; Success&lt;/p&gt; 
+&lt;p class="status-text"&gt;&lt;strong&gt;Uploader ID:&lt;/strong&gt; {0}&lt;/p&gt; 
 &lt;div class="table-container"&gt;
+  &lt;strong&gt;1. Dispute Submission Statistics&lt;/strong&gt;
   &lt;table&gt;
     &lt;thead&gt;
       &lt;tr&gt;
-        &lt;th&gt;BOT Run Statistics&lt;/th&gt;
+        &lt;th&gt;Category&lt;/th&gt;
         &lt;th class="count-col"&gt;Count&lt;/th&gt;
       &lt;/tr&gt;
     &lt;/thead&gt;
     &lt;tbody&gt;
       &lt;tr&gt;
-        &lt;td&gt;Total No of records processed in the run&lt;/td&gt;
-        &lt;td&gt;5&lt;/td&gt;
+        &lt;td&gt;Total Records Processed&lt;/td&gt;
+        &lt;td class="count-col"&gt;{1}&lt;/td&gt;
       &lt;/tr&gt;
       &lt;tr&gt;
-        &lt;td&gt;No of records processed Successfully&lt;/td&gt;
-        &lt;td&gt;3&lt;/td&gt;
+        &lt;td&gt;Successful Submissions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{2}&lt;/td&gt;
       &lt;/tr&gt;
       &lt;tr&gt;
-        &lt;td&gt;No of business exceptions&lt;/td&gt;
-        &lt;td&gt;1&lt;/td&gt;
-      &lt;/tr&gt;
-      &lt;tr&gt;
-        &lt;td&gt;No of system exceptions&lt;/td&gt;
-        &lt;td&gt;1&lt;/td&gt;
+        &lt;td&gt;Success Percentage&lt;/td&gt;
+        &lt;td class="count-col"&gt;{3}%&lt;/td&gt;
       &lt;/tr&gt;
     &lt;/tbody&gt;
   &lt;/table&gt;
 &lt;/div&gt;
+&lt;div class="table-container"&gt;
+  &lt;strong&gt;2. Exception Breakdown&lt;/strong&gt;
+  &lt;table&gt;
+    &lt;thead&gt;
+      &lt;tr&gt;
+        &lt;th&gt;Exception Type&lt;/th&gt;
+        &lt;th class="count-col"&gt;Count&lt;/th&gt;
+      &lt;/tr&gt;
+    &lt;/thead&gt;
+    &lt;tbody&gt;
+      &lt;tr&gt;
+        &lt;td&gt;Business Exceptions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{4}&lt;/td&gt;
+      &lt;/tr&gt;
+      &lt;tr&gt;
+        &lt;td&gt;System Exceptions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{5}&lt;/td&gt;
+      &lt;/tr&gt;
+    &lt;/tbody&gt;
+  &lt;/table&gt;
+&lt;/div&gt;
+&lt;p&gt;Please find the attachment of the consolidated log table for your reference.&lt;/p&gt;
 &lt;p&gt;Thanks,&lt;br&gt;
 &lt;strong&gt;RPA Team&lt;/strong&gt;&lt;/p&gt;
 &lt;/body&gt;
 &lt;/html&gt;</t>
   </si>
   <si>
-    <t>SuccessDisputeMailBody</t>
-  </si>
-  <si>
-    <t>SuccessDisputeMailSubject</t>
-  </si>
-  <si>
-    <t>ArchiveSavedBatch</t>
-  </si>
-  <si>
-    <t>TaregtAsanaUserID</t>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html&gt;
+&lt;head&gt;
+&lt;style&gt;
+  body { font-family: Arial, sans-serif; font-size: 14px; color: #333333; line-height: 1.5; }
+  .table-container { margin-top: 15px; margin-bottom: 20px; }
+  table { border-collapse: collapse; width: 450px; font-size: 13px; }
+  th { background-color: #f2f2f2; text-align: left; font-weight: bold; padding: 8px; border: 1px solid #999999; }
+  td { padding: 8px; border: 1px solid #999999; }
+  .count-col { width: 100px; text-align: center; }
+  .status-text { font-family: Arial, sans-serif; font-size: 14px; margin: 10px 0; }
+&lt;/style&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;p&gt;Hi Team,&lt;/p&gt;
+&lt;p class="status-text"&gt;Please find below the &lt;strong&gt;Dispute Process Summary&lt;/strong&gt; of the claims processed in this bot run.&lt;/p&gt; 
+&lt;p class="status-text"&gt;&lt;strong&gt;Uploader Step:&lt;/strong&gt;Error Occured in the creation and running the CSV file for Claim Uploader. This step will need to be completed manually, please contact IT to get an understanding of the exception&lt;/p&gt; 
+&lt;p class="status-text"&gt;&lt;strong&gt;Uploader ID:&lt;/strong&gt; {0}&lt;/p&gt; 
+&lt;div class="table-container"&gt;
+  &lt;strong&gt;1. Dispute Submission Statistics&lt;/strong&gt;
+  &lt;table&gt;
+    &lt;thead&gt;
+      &lt;tr&gt;
+        &lt;th&gt;Category&lt;/th&gt;
+        &lt;th class="count-col"&gt;Count&lt;/th&gt;
+      &lt;/tr&gt;
+    &lt;/thead&gt;
+    &lt;tbody&gt;
+      &lt;tr&gt;
+        &lt;td&gt;Total Records Processed&lt;/td&gt;
+        &lt;td class="count-col"&gt;{1}&lt;/td&gt;
+      &lt;/tr&gt;
+      &lt;tr&gt;
+        &lt;td&gt;Successful Submissions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{2}&lt;/td&gt;
+      &lt;/tr&gt;
+      &lt;tr&gt;
+        &lt;td&gt;Success Percentage&lt;/td&gt;
+        &lt;td class="count-col"&gt;{3}%&lt;/td&gt;
+      &lt;/tr&gt;
+    &lt;/tbody&gt;
+  &lt;/table&gt;
+&lt;/div&gt;
+&lt;div class="table-container"&gt;
+  &lt;strong&gt;2. Exception Breakdown&lt;/strong&gt;
+  &lt;table&gt;
+    &lt;thead&gt;
+      &lt;tr&gt;
+        &lt;th&gt;Exception Type&lt;/th&gt;
+        &lt;th class="count-col"&gt;Count&lt;/th&gt;
+      &lt;/tr&gt;
+    &lt;/thead&gt;
+    &lt;tbody&gt;
+      &lt;tr&gt;
+        &lt;td&gt;Business Exceptions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{4}&lt;/td&gt;
+      &lt;/tr&gt;
+      &lt;tr&gt;
+        &lt;td&gt;System Exceptions&lt;/td&gt;
+        &lt;td class="count-col"&gt;{5}&lt;/td&gt;
+      &lt;/tr&gt;
+    &lt;/tbody&gt;
+  &lt;/table&gt;
+&lt;/div&gt;
+&lt;p&gt;Please find the attachment of the consolidated log table for your reference.&lt;/p&gt;
+&lt;p&gt;Thanks,&lt;br&gt;
+&lt;strong&gt;RPA Team&lt;/strong&gt;&lt;/p&gt;
+&lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>DisputeOracleFileUpload</t>
+  </si>
+  <si>
+    <t>DisputeOracleProgramName</t>
+  </si>
+  <si>
+    <t>LOGI Transactions Uploader in AR with Lex field Datapoints</t>
+  </si>
+  <si>
+    <t>LOGI_TRX_DATAPOINT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -652,6 +963,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -688,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -708,6 +1025,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,409 +1341,447 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z957"/>
+  <dimension ref="A1:B951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="30">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A11" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
+    </row>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+    <row r="13" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A13" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>117</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
         <v>118</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
         <v>119</v>
       </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>126</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="B28" s="9"/>
     </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43">
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>159</v>
-      </c>
-      <c r="B41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
       <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>176</v>
+      </c>
+      <c r="B49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="2" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A52" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A48" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
-        <v>138</v>
-      </c>
-      <c r="B53" t="s">
-        <v>139</v>
-      </c>
-    </row>
+      <c r="B52" s="10">
+        <v>1210009146617350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>164</v>
-      </c>
-      <c r="B58" s="10">
-        <v>1210009146617350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>165</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" t="s">
+        <v>172</v>
+      </c>
+    </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -2297,12 +2653,6 @@
     <row r="949" ht="14.25" customHeight="1"/>
     <row r="950" ht="14.25" customHeight="1"/>
     <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2323,217 +2673,217 @@
   <sheetData>
     <row r="1" spans="1:71">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>54</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>55</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>56</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>57</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>59</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>63</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>64</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>65</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>67</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>68</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>69</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>70</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>72</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>73</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>74</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>75</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>76</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>77</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>78</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>79</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>81</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>82</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>83</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>84</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>85</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>86</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>87</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>88</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>90</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>91</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>92</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>93</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>94</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>95</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>96</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>97</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>98</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>99</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>100</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>101</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>102</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>103</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>104</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>105</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>106</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2624,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2646,7 +2996,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -2657,7 +3007,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -2668,7 +3018,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3679,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>